<commit_message>
Edit and re export DD Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/DDGantt.xlsx
+++ b/pp/gantt/DDGantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Davide, Mario, Moreno</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Definition of system boundaries</t>
   </si>
   <si>
-    <t>High level system view</t>
-  </si>
-  <si>
     <t>Architecture draft</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>Task #</t>
+  </si>
+  <si>
+    <t>High level system view definition</t>
+  </si>
+  <si>
+    <t>Moreno will start working on this activity in date 29/11/2016</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,31 +508,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -537,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F2,G2),"g")</f>
+        <f t="shared" ref="E2:E18" si="0">CONCATENATE(NETWORKDAYS(F2,G2),"g")</f>
         <v>20g</v>
       </c>
       <c r="F2" s="1">
@@ -561,13 +564,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F3,G3),"g")</f>
+        <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="F3" s="1">
@@ -585,13 +588,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F4,G4),"g")</f>
+        <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="F4" s="1">
@@ -615,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F5,G5),"g")</f>
+        <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="F5" s="1">
@@ -640,7 +643,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F6,G6),"g")</f>
+        <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="F6" s="1">
@@ -664,14 +667,14 @@
         <v>0</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F7,G7),"g")</f>
-        <v>2g</v>
+        <f t="shared" si="0"/>
+        <v>1g</v>
       </c>
       <c r="F7" s="1">
         <v>42691.333333333336</v>
       </c>
       <c r="G7" s="1">
-        <v>42692.666666666664</v>
+        <v>42691.666666666664</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -688,14 +691,14 @@
         <v>0</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F8,G8),"g")</f>
-        <v>3g</v>
+        <f t="shared" si="0"/>
+        <v>2g</v>
       </c>
       <c r="F8" s="1">
-        <v>42695.333333333336</v>
+        <v>42692.333333333336</v>
       </c>
       <c r="G8" s="1">
-        <v>42697.666666666664</v>
+        <v>42695.666666666664</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -712,14 +715,14 @@
         <v>0</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F9,G9),"g")</f>
-        <v>3g</v>
+        <f t="shared" si="0"/>
+        <v>2g</v>
       </c>
       <c r="F9" s="1">
-        <v>42698.333333333336</v>
+        <v>42696.333333333336</v>
       </c>
       <c r="G9" s="1">
-        <v>42702.666666666664</v>
+        <v>42697.666666666664</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -730,20 +733,20 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E10" t="str">
         <f>CONCATENATE(NETWORKDAYS(F10,G10),"g")</f>
-        <v>2g</v>
+        <v>1g</v>
       </c>
       <c r="F10" s="1">
-        <v>42703.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="G10" s="1">
-        <v>42704.666666666664</v>
+        <v>42698.666666666664</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -754,20 +757,20 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E11" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F11,G11),"g")</f>
-        <v>3g</v>
+        <f t="shared" si="0"/>
+        <v>2g</v>
       </c>
       <c r="F11" s="1">
-        <v>42703.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="G11" s="1">
-        <v>42705.666666666664</v>
+        <v>42699.666666666664</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -784,14 +787,14 @@
         <v>6</v>
       </c>
       <c r="E12" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F12,G12),"g")</f>
+        <f t="shared" si="0"/>
         <v>2g</v>
       </c>
       <c r="F12" s="1">
-        <v>42703.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="G12" s="1">
-        <v>42704.666666666664</v>
+        <v>42699.666666666664</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -802,20 +805,23 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
       </c>
       <c r="E13" t="str">
         <f>CONCATENATE(NETWORKDAYS(F13,G13),"g")</f>
-        <v>1g</v>
+        <v>4g</v>
       </c>
       <c r="F13" s="1">
-        <v>42705.333333333336</v>
+        <v>42699.333333333336</v>
       </c>
       <c r="G13" s="1">
-        <v>42705.666666666664</v>
+        <v>42704.666666666664</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -826,20 +832,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F14,G14),"g")</f>
-        <v>3g</v>
+        <f t="shared" si="0"/>
+        <v>1g</v>
       </c>
       <c r="F14" s="1">
-        <v>42706.333333333336</v>
+        <v>42702.333333333336</v>
       </c>
       <c r="G14" s="1">
-        <v>42710.666666666664</v>
+        <v>42702.666666666664</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -856,14 +862,14 @@
         <v>6</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F15,G15),"g")</f>
-        <v>3g</v>
+        <f t="shared" si="0"/>
+        <v>2g</v>
       </c>
       <c r="F15" s="1">
-        <v>42706.333333333336</v>
+        <v>42703.333333333336</v>
       </c>
       <c r="G15" s="1">
-        <v>42710.666666666664</v>
+        <v>42704.666666666664</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -881,14 +887,14 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F16,G16),"g")</f>
+        <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="F16" s="1">
-        <v>42711.333333333336</v>
+        <v>42705.333333333336</v>
       </c>
       <c r="G16" s="1">
-        <v>42711.666666666664</v>
+        <v>42705.666666666664</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -905,14 +911,14 @@
         <v>2</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F17,G17),"g")</f>
+        <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="F17" s="1">
-        <v>42711.333333333336</v>
+        <v>42705.333333333336</v>
       </c>
       <c r="G17" s="1">
-        <v>42711.666666666664</v>
+        <v>42705.666666666664</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -929,14 +935,14 @@
         <v>0</v>
       </c>
       <c r="E18" t="str">
-        <f>CONCATENATE(NETWORKDAYS(F18,G18),"g")</f>
+        <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="F18" s="1">
-        <v>42713.333333333336</v>
+        <v>42706.333333333336</v>
       </c>
       <c r="G18" s="1">
-        <v>42713.666666666664</v>
+        <v>42706.666666666664</v>
       </c>
       <c r="I18">
         <v>2</v>

</xml_diff>